<commit_message>
Nå er deltakerliste slik som vi ønsker
</commit_message>
<xml_diff>
--- a/Deltakerliste - KUNSTLØP_ Oppvisning Bergen.xlsx
+++ b/Deltakerliste - KUNSTLØP_ Oppvisning Bergen.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ27"/>
+  <dimension ref="A1:AQ25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2629,39 +2629,39 @@
         <v>Ja</v>
       </c>
     </row>
-    <row r="18" xml:space="preserve">
+    <row r="18">
       <c r="A18" t="str">
-        <v>Mina</v>
+        <v>Eira Olava Bortne</v>
       </c>
       <c r="B18" t="str">
-        <v>Lam</v>
+        <v>Ludvigsen</v>
       </c>
       <c r="C18" t="str">
-        <v>posten1428@gmail.com</v>
+        <v>ssludvigsen@gmail.com</v>
       </c>
       <c r="D18" t="str">
-        <v>Norge</v>
+        <v/>
       </c>
       <c r="E18" t="str">
-        <v>NOR</v>
+        <v/>
       </c>
       <c r="F18" t="str">
-        <v>09.08.2012</v>
+        <v>18.04.2016</v>
       </c>
       <c r="G18" t="str">
-        <v>13 år</v>
+        <v>9 år</v>
       </c>
       <c r="H18" t="str">
-        <v>+4791852489</v>
+        <v>+4741322734</v>
       </c>
       <c r="I18" t="str">
         <v>K</v>
       </c>
       <c r="J18" t="str">
-        <v>Loddefjord IL</v>
+        <v>Bergen Kunstløpklubb</v>
       </c>
       <c r="K18" t="str">
-        <v>24878</v>
+        <v>24787</v>
       </c>
       <c r="L18" t="str">
         <v/>
@@ -2679,7 +2679,7 @@
         <v/>
       </c>
       <c r="Q18" t="str">
-        <v/>
+        <v xml:space="preserve">Oppvisning Reg.3 Vestlandet og Sørlandet </v>
       </c>
       <c r="R18" t="str">
         <v/>
@@ -2691,25 +2691,25 @@
         <v>17:00</v>
       </c>
       <c r="U18" t="str">
-        <v/>
+        <v>305</v>
       </c>
       <c r="V18" t="str">
-        <v/>
+        <v>0</v>
       </c>
       <c r="W18" t="str">
-        <v>N</v>
+        <v>J</v>
       </c>
       <c r="X18" t="str">
-        <v/>
+        <v>d1d51orf00006n01qci0</v>
       </c>
       <c r="Y18" t="str">
         <v/>
       </c>
       <c r="Z18" t="str">
-        <v>Thai Quang Lam</v>
+        <v>Stian Skår Ludvigsen</v>
       </c>
       <c r="AA18" t="str">
-        <v>posten1428@gmail.com</v>
+        <v>ssludvigsen@gmail.com</v>
       </c>
       <c r="AB18" t="str">
         <v>305</v>
@@ -2721,32 +2721,31 @@
         <v>Ja</v>
       </c>
       <c r="AE18" t="str">
-        <v>37276205156</v>
+        <v>37276312297</v>
       </c>
       <c r="AF18" t="str">
-        <v>cmkd04cnv035icy01hkthrr18</v>
+        <v>cmkd0b10n034kgl010yoac2gk</v>
       </c>
       <c r="AG18" t="str">
-        <v>Avmeldt</v>
+        <v>Påmeldt</v>
       </c>
       <c r="AH18" t="str">
         <v>13.01.2026</v>
       </c>
       <c r="AI18" t="str">
-        <v>20:45</v>
+        <v>20:50</v>
       </c>
       <c r="AJ18" t="str">
-        <v>Avmeldt</v>
-      </c>
-      <c r="AK18" t="str" xml:space="preserve">
-        <v xml:space="preserve">Betaling nr: 1 (PAID) Beløp: 305,- 
-Betaling nr: 2 (PAID) Beløp: -305,-</v>
+        <v>Ikke sjekket inn</v>
+      </c>
+      <c r="AK18" t="str">
+        <v>Betaling nr: 1 (PAID) Beløp: 305,-</v>
       </c>
       <c r="AL18" t="str">
         <v>000000000</v>
       </c>
       <c r="AM18" t="str">
-        <v>9491192</v>
+        <v>10210494</v>
       </c>
       <c r="AN18" t="str">
         <v/>
@@ -2763,28 +2762,28 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Eira Olava Bortne</v>
+        <v>Sara Barbro</v>
       </c>
       <c r="B19" t="str">
-        <v>Ludvigsen</v>
+        <v>Kyte</v>
       </c>
       <c r="C19" t="str">
-        <v>ssludvigsen@gmail.com</v>
+        <v>vibeke.vold@gmail.com</v>
       </c>
       <c r="D19" t="str">
-        <v/>
+        <v>Norge</v>
       </c>
       <c r="E19" t="str">
-        <v/>
+        <v>NOR</v>
       </c>
       <c r="F19" t="str">
-        <v>18.04.2016</v>
+        <v>04.08.2016</v>
       </c>
       <c r="G19" t="str">
         <v>9 år</v>
       </c>
       <c r="H19" t="str">
-        <v>+4741322734</v>
+        <v>+4790013289</v>
       </c>
       <c r="I19" t="str">
         <v>K</v>
@@ -2838,10 +2837,10 @@
         <v/>
       </c>
       <c r="Z19" t="str">
-        <v>Stian Skår Ludvigsen</v>
+        <v>Sara Barbro Kyte</v>
       </c>
       <c r="AA19" t="str">
-        <v>ssludvigsen@gmail.com</v>
+        <v>vibeke.vold@gmail.com</v>
       </c>
       <c r="AB19" t="str">
         <v>305</v>
@@ -2853,10 +2852,10 @@
         <v>Ja</v>
       </c>
       <c r="AE19" t="str">
-        <v>37276312297</v>
+        <v>37277878945</v>
       </c>
       <c r="AF19" t="str">
-        <v>cmkd0b10n034kgl010yoac2gk</v>
+        <v>cmkd2r7kw03u6cy0163qqpurt</v>
       </c>
       <c r="AG19" t="str">
         <v>Påmeldt</v>
@@ -2865,7 +2864,7 @@
         <v>13.01.2026</v>
       </c>
       <c r="AI19" t="str">
-        <v>20:50</v>
+        <v>21:59</v>
       </c>
       <c r="AJ19" t="str">
         <v>Ikke sjekket inn</v>
@@ -2874,10 +2873,10 @@
         <v>Betaling nr: 1 (PAID) Beløp: 305,-</v>
       </c>
       <c r="AL19" t="str">
-        <v>000000000</v>
+        <v>146874367</v>
       </c>
       <c r="AM19" t="str">
-        <v>10210494</v>
+        <v>9456484</v>
       </c>
       <c r="AN19" t="str">
         <v/>
@@ -2894,40 +2893,40 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Sara Barbro</v>
+        <v>Mille Isabell</v>
       </c>
       <c r="B20" t="str">
-        <v>Kyte</v>
+        <v>Steen Rein</v>
       </c>
       <c r="C20" t="str">
-        <v>vibeke.vold@gmail.com</v>
+        <v>moniq_82@hotmail.com</v>
       </c>
       <c r="D20" t="str">
-        <v>Norge</v>
+        <v/>
       </c>
       <c r="E20" t="str">
-        <v>NOR</v>
+        <v/>
       </c>
       <c r="F20" t="str">
-        <v>04.08.2016</v>
+        <v>26.08.2016</v>
       </c>
       <c r="G20" t="str">
         <v>9 år</v>
       </c>
       <c r="H20" t="str">
-        <v>+4790013289</v>
+        <v>91162897</v>
       </c>
       <c r="I20" t="str">
         <v>K</v>
       </c>
       <c r="J20" t="str">
-        <v>Bergen Kunstløpklubb</v>
+        <v>Loddefjord IL</v>
       </c>
       <c r="K20" t="str">
-        <v>24787</v>
+        <v>24878</v>
       </c>
       <c r="L20" t="str">
-        <v/>
+        <v>610594</v>
       </c>
       <c r="M20" t="str">
         <v>Hordaland Skøytekrets</v>
@@ -2960,19 +2959,19 @@
         <v>0</v>
       </c>
       <c r="W20" t="str">
-        <v>J</v>
+        <v>N</v>
       </c>
       <c r="X20" t="str">
-        <v>d1d51orf00006n01qci0</v>
+        <v/>
       </c>
       <c r="Y20" t="str">
         <v/>
       </c>
       <c r="Z20" t="str">
-        <v>Sara Barbro Kyte</v>
+        <v>Anja Papenbrock Bjarndisson</v>
       </c>
       <c r="AA20" t="str">
-        <v>vibeke.vold@gmail.com</v>
+        <v>apapenbrock@gmx.de</v>
       </c>
       <c r="AB20" t="str">
         <v>305</v>
@@ -2984,19 +2983,19 @@
         <v>Ja</v>
       </c>
       <c r="AE20" t="str">
-        <v>37277878945</v>
+        <v/>
       </c>
       <c r="AF20" t="str">
-        <v>cmkd2r7kw03u6cy0163qqpurt</v>
+        <v>cmkdxpv8200eqc9017ts3odpp</v>
       </c>
       <c r="AG20" t="str">
         <v>Påmeldt</v>
       </c>
       <c r="AH20" t="str">
-        <v>13.01.2026</v>
+        <v>14.01.2026</v>
       </c>
       <c r="AI20" t="str">
-        <v>21:59</v>
+        <v>13:45</v>
       </c>
       <c r="AJ20" t="str">
         <v>Ikke sjekket inn</v>
@@ -3005,10 +3004,10 @@
         <v>Betaling nr: 1 (PAID) Beløp: 305,-</v>
       </c>
       <c r="AL20" t="str">
-        <v>146874367</v>
+        <v/>
       </c>
       <c r="AM20" t="str">
-        <v>9456484</v>
+        <v/>
       </c>
       <c r="AN20" t="str">
         <v/>
@@ -3017,45 +3016,45 @@
         <v/>
       </c>
       <c r="AP20" t="str">
-        <v>Ja</v>
+        <v>Nei</v>
       </c>
       <c r="AQ20" t="str">
-        <v>Ja</v>
+        <v>Nei</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v xml:space="preserve">Oda Eilin </v>
+        <v>Yuewei</v>
       </c>
       <c r="B21" t="str">
-        <v>Halkjelsvik-Sæbø</v>
+        <v>Li</v>
       </c>
       <c r="C21" t="str">
-        <v>Renatehal@hotmail.com</v>
+        <v>youran.y@gmail.com</v>
       </c>
       <c r="D21" t="str">
-        <v>Norge</v>
+        <v>Kina</v>
       </c>
       <c r="E21" t="str">
-        <v>NOR</v>
+        <v>CHN</v>
       </c>
       <c r="F21" t="str">
-        <v>31.03.2017</v>
+        <v>03.10.2016</v>
       </c>
       <c r="G21" t="str">
-        <v>8 år</v>
+        <v>9 år</v>
       </c>
       <c r="H21" t="str">
-        <v>+4747307450</v>
+        <v>+4747167293</v>
       </c>
       <c r="I21" t="str">
         <v>K</v>
       </c>
       <c r="J21" t="str">
-        <v>Fana Idrettslag</v>
+        <v>Bergen Kunstløpklubb</v>
       </c>
       <c r="K21" t="str">
-        <v>24834</v>
+        <v>24787</v>
       </c>
       <c r="L21" t="str">
         <v/>
@@ -3073,7 +3072,7 @@
         <v/>
       </c>
       <c r="Q21" t="str">
-        <v/>
+        <v xml:space="preserve">Oppvisning Reg.3 Vestlandet og Sørlandet </v>
       </c>
       <c r="R21" t="str">
         <v/>
@@ -3085,28 +3084,28 @@
         <v>17:00</v>
       </c>
       <c r="U21" t="str">
-        <v/>
+        <v>305</v>
       </c>
       <c r="V21" t="str">
-        <v/>
+        <v>0</v>
       </c>
       <c r="W21" t="str">
-        <v>N</v>
+        <v>J</v>
       </c>
       <c r="X21" t="str">
-        <v/>
+        <v>d1d51orf00006n01qci0</v>
       </c>
       <c r="Y21" t="str">
         <v/>
       </c>
       <c r="Z21" t="str">
-        <v>Renate Kristin Halkjelsvik</v>
+        <v>Yuewei Li</v>
       </c>
       <c r="AA21" t="str">
-        <v>Renatehal@hotmail.com</v>
+        <v>youran.y@gmail.com</v>
       </c>
       <c r="AB21" t="str">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="AC21" t="str">
         <v>0</v>
@@ -3115,31 +3114,31 @@
         <v>Ja</v>
       </c>
       <c r="AE21" t="str">
-        <v>37279442547</v>
+        <v>37294517184</v>
       </c>
       <c r="AF21" t="str">
-        <v>cmkd588xe044tb901bmqzpr6o</v>
+        <v>cmkee81w60191bs015t79k1d1</v>
       </c>
       <c r="AG21" t="str">
-        <v>Avmeldt</v>
+        <v>Påmeldt</v>
       </c>
       <c r="AH21" t="str">
-        <v>13.01.2026</v>
+        <v>14.01.2026</v>
       </c>
       <c r="AI21" t="str">
-        <v>23:08</v>
+        <v>20:07</v>
       </c>
       <c r="AJ21" t="str">
-        <v>Avmeldt</v>
+        <v>Ikke sjekket inn</v>
       </c>
       <c r="AK21" t="str">
-        <v>Betaling nr: 1 (PAID) Beløp: 310,-</v>
+        <v>Betaling nr: 1 (PAID) Beløp: 305,-</v>
       </c>
       <c r="AL21" t="str">
-        <v>000000000</v>
+        <v>137247243</v>
       </c>
       <c r="AM21" t="str">
-        <v>10459939</v>
+        <v>9077466</v>
       </c>
       <c r="AN21" t="str">
         <v/>
@@ -3148,7 +3147,7 @@
         <v/>
       </c>
       <c r="AP21" t="str">
-        <v>Ja</v>
+        <v>Nei</v>
       </c>
       <c r="AQ21" t="str">
         <v>Ja</v>
@@ -3156,28 +3155,28 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Mille Isabell</v>
+        <v>Eleanora</v>
       </c>
       <c r="B22" t="str">
-        <v>Steen Rein</v>
+        <v>Egle</v>
       </c>
       <c r="C22" t="str">
-        <v>moniq_82@hotmail.com</v>
+        <v>liva.egle@gmail.com</v>
       </c>
       <c r="D22" t="str">
-        <v/>
+        <v>Latvia</v>
       </c>
       <c r="E22" t="str">
-        <v/>
+        <v>LAT</v>
       </c>
       <c r="F22" t="str">
-        <v>26.08.2016</v>
+        <v>25.07.2016</v>
       </c>
       <c r="G22" t="str">
         <v>9 år</v>
       </c>
       <c r="H22" t="str">
-        <v>91162897</v>
+        <v>+4792552135</v>
       </c>
       <c r="I22" t="str">
         <v>K</v>
@@ -3189,7 +3188,7 @@
         <v>24878</v>
       </c>
       <c r="L22" t="str">
-        <v>610594</v>
+        <v/>
       </c>
       <c r="M22" t="str">
         <v>Hordaland Skøytekrets</v>
@@ -3222,19 +3221,19 @@
         <v>0</v>
       </c>
       <c r="W22" t="str">
-        <v>N</v>
+        <v>J</v>
       </c>
       <c r="X22" t="str">
-        <v/>
+        <v>d1d51orf00006n01qci0</v>
       </c>
       <c r="Y22" t="str">
         <v/>
       </c>
       <c r="Z22" t="str">
-        <v>Anja Papenbrock Bjarndisson</v>
+        <v>Liva Egle</v>
       </c>
       <c r="AA22" t="str">
-        <v>apapenbrock@gmx.de</v>
+        <v>liva.egle@gmail.com</v>
       </c>
       <c r="AB22" t="str">
         <v>305</v>
@@ -3246,19 +3245,19 @@
         <v>Ja</v>
       </c>
       <c r="AE22" t="str">
-        <v/>
+        <v>37320124633</v>
       </c>
       <c r="AF22" t="str">
-        <v>cmkdxpv8200eqc9017ts3odpp</v>
+        <v>cmkghbrqj0021cz01891mf9em</v>
       </c>
       <c r="AG22" t="str">
         <v>Påmeldt</v>
       </c>
       <c r="AH22" t="str">
-        <v>14.01.2026</v>
+        <v>16.01.2026</v>
       </c>
       <c r="AI22" t="str">
-        <v>13:45</v>
+        <v>07:10</v>
       </c>
       <c r="AJ22" t="str">
         <v>Ikke sjekket inn</v>
@@ -3267,10 +3266,10 @@
         <v>Betaling nr: 1 (PAID) Beløp: 305,-</v>
       </c>
       <c r="AL22" t="str">
-        <v/>
+        <v>000000000</v>
       </c>
       <c r="AM22" t="str">
-        <v/>
+        <v>9639788</v>
       </c>
       <c r="AN22" t="str">
         <v/>
@@ -3282,42 +3281,42 @@
         <v>Nei</v>
       </c>
       <c r="AQ22" t="str">
-        <v>Nei</v>
+        <v>Ja</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Yuewei</v>
+        <v>Angela</v>
       </c>
       <c r="B23" t="str">
-        <v>Li</v>
+        <v>Chen</v>
       </c>
       <c r="C23" t="str">
-        <v>youran.y@gmail.com</v>
+        <v>kchen3997@gmail.com</v>
       </c>
       <c r="D23" t="str">
-        <v>Kina</v>
+        <v>Norge</v>
       </c>
       <c r="E23" t="str">
-        <v>CHN</v>
+        <v>NOR</v>
       </c>
       <c r="F23" t="str">
-        <v>03.10.2016</v>
+        <v>09.10.2016</v>
       </c>
       <c r="G23" t="str">
         <v>9 år</v>
       </c>
       <c r="H23" t="str">
-        <v>+4747167293</v>
+        <v>+4794024593</v>
       </c>
       <c r="I23" t="str">
         <v>K</v>
       </c>
       <c r="J23" t="str">
-        <v>Bergen Kunstløpklubb</v>
+        <v>Fana Idrettslag</v>
       </c>
       <c r="K23" t="str">
-        <v>24787</v>
+        <v>24834</v>
       </c>
       <c r="L23" t="str">
         <v/>
@@ -3362,10 +3361,10 @@
         <v/>
       </c>
       <c r="Z23" t="str">
-        <v>Yuewei Li</v>
+        <v>Kang Chen</v>
       </c>
       <c r="AA23" t="str">
-        <v>youran.y@gmail.com</v>
+        <v>kchen3997@gmail.com</v>
       </c>
       <c r="AB23" t="str">
         <v>305</v>
@@ -3377,19 +3376,19 @@
         <v>Ja</v>
       </c>
       <c r="AE23" t="str">
-        <v>37294517184</v>
+        <v>37367115886</v>
       </c>
       <c r="AF23" t="str">
-        <v>cmkee81w60191bs015t79k1d1</v>
+        <v>cmkk3tb7a061qcx0137352zdc</v>
       </c>
       <c r="AG23" t="str">
         <v>Påmeldt</v>
       </c>
       <c r="AH23" t="str">
-        <v>14.01.2026</v>
+        <v>18.01.2026</v>
       </c>
       <c r="AI23" t="str">
-        <v>20:07</v>
+        <v>20:03</v>
       </c>
       <c r="AJ23" t="str">
         <v>Ikke sjekket inn</v>
@@ -3398,10 +3397,10 @@
         <v>Betaling nr: 1 (PAID) Beløp: 305,-</v>
       </c>
       <c r="AL23" t="str">
-        <v>137247243</v>
+        <v>000000000</v>
       </c>
       <c r="AM23" t="str">
-        <v>9077466</v>
+        <v>9865886</v>
       </c>
       <c r="AN23" t="str">
         <v/>
@@ -3410,7 +3409,7 @@
         <v/>
       </c>
       <c r="AP23" t="str">
-        <v>Nei</v>
+        <v>Ja</v>
       </c>
       <c r="AQ23" t="str">
         <v>Ja</v>
@@ -3418,37 +3417,37 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Eleanora</v>
+        <v>Aurelia</v>
       </c>
       <c r="B24" t="str">
-        <v>Egle</v>
+        <v>Landschulze</v>
       </c>
       <c r="C24" t="str">
-        <v>liva.egle@gmail.com</v>
+        <v>klandschulze@posteo.no</v>
       </c>
       <c r="D24" t="str">
-        <v>Latvia</v>
+        <v>Tyskland</v>
       </c>
       <c r="E24" t="str">
-        <v>LAT</v>
+        <v>GER</v>
       </c>
       <c r="F24" t="str">
-        <v>25.07.2016</v>
+        <v>10.04.2015</v>
       </c>
       <c r="G24" t="str">
-        <v>9 år</v>
+        <v>10 år</v>
       </c>
       <c r="H24" t="str">
-        <v>+4792552135</v>
+        <v>+4740646286</v>
       </c>
       <c r="I24" t="str">
         <v>K</v>
       </c>
       <c r="J24" t="str">
-        <v>Loddefjord IL</v>
+        <v>Fana Idrettslag</v>
       </c>
       <c r="K24" t="str">
-        <v>24878</v>
+        <v>24834</v>
       </c>
       <c r="L24" t="str">
         <v/>
@@ -3493,10 +3492,10 @@
         <v/>
       </c>
       <c r="Z24" t="str">
-        <v>Liva Egle</v>
+        <v>Karin Landschulze</v>
       </c>
       <c r="AA24" t="str">
-        <v>liva.egle@gmail.com</v>
+        <v>klandschulze@posteo.no</v>
       </c>
       <c r="AB24" t="str">
         <v>305</v>
@@ -3508,19 +3507,19 @@
         <v>Ja</v>
       </c>
       <c r="AE24" t="str">
-        <v>37320124633</v>
+        <v>37380862685</v>
       </c>
       <c r="AF24" t="str">
-        <v>cmkghbrqj0021cz01891mf9em</v>
+        <v>cmklbsxxg00jycg01s2378t65</v>
       </c>
       <c r="AG24" t="str">
         <v>Påmeldt</v>
       </c>
       <c r="AH24" t="str">
-        <v>16.01.2026</v>
+        <v>19.01.2026</v>
       </c>
       <c r="AI24" t="str">
-        <v>07:10</v>
+        <v>16:34</v>
       </c>
       <c r="AJ24" t="str">
         <v>Ikke sjekket inn</v>
@@ -3532,7 +3531,7 @@
         <v>000000000</v>
       </c>
       <c r="AM24" t="str">
-        <v>9639788</v>
+        <v>9583455</v>
       </c>
       <c r="AN24" t="str">
         <v/>
@@ -3541,7 +3540,7 @@
         <v/>
       </c>
       <c r="AP24" t="str">
-        <v>Nei</v>
+        <v>Ja</v>
       </c>
       <c r="AQ24" t="str">
         <v>Ja</v>
@@ -3549,40 +3548,40 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Angela</v>
+        <v>Leah</v>
       </c>
       <c r="B25" t="str">
-        <v>Chen</v>
+        <v>Kalvik</v>
       </c>
       <c r="C25" t="str">
-        <v>kchen3997@gmail.com</v>
+        <v>per.asle.sandal@gmail.com</v>
       </c>
       <c r="D25" t="str">
-        <v>Norge</v>
+        <v>NO</v>
       </c>
       <c r="E25" t="str">
-        <v>NOR</v>
+        <v/>
       </c>
       <c r="F25" t="str">
-        <v>09.10.2016</v>
+        <v>08.09.2014</v>
       </c>
       <c r="G25" t="str">
-        <v>9 år</v>
+        <v>11 år</v>
       </c>
       <c r="H25" t="str">
-        <v>+4794024593</v>
+        <v>+4741678027</v>
       </c>
       <c r="I25" t="str">
         <v>K</v>
       </c>
       <c r="J25" t="str">
-        <v>Fana Idrettslag</v>
+        <v>Loddefjord IL</v>
       </c>
       <c r="K25" t="str">
-        <v>24834</v>
+        <v>24878</v>
       </c>
       <c r="L25" t="str">
-        <v/>
+        <v>610594</v>
       </c>
       <c r="M25" t="str">
         <v>Hordaland Skøytekrets</v>
@@ -3597,7 +3596,7 @@
         <v/>
       </c>
       <c r="Q25" t="str">
-        <v xml:space="preserve">Oppvisning Reg.3 Vestlandet og Sørlandet </v>
+        <v/>
       </c>
       <c r="R25" t="str">
         <v/>
@@ -3609,61 +3608,61 @@
         <v>17:00</v>
       </c>
       <c r="U25" t="str">
-        <v>305</v>
+        <v/>
       </c>
       <c r="V25" t="str">
-        <v>0</v>
+        <v/>
       </c>
       <c r="W25" t="str">
-        <v>J</v>
+        <v>N</v>
       </c>
       <c r="X25" t="str">
-        <v>d1d51orf00006n01qci0</v>
+        <v/>
       </c>
       <c r="Y25" t="str">
         <v/>
       </c>
       <c r="Z25" t="str">
-        <v>Kang Chen</v>
+        <v>Anja Papenbrock Bjarndisson</v>
       </c>
       <c r="AA25" t="str">
-        <v>kchen3997@gmail.com</v>
+        <v>apapenbrock@gmx.de</v>
       </c>
       <c r="AB25" t="str">
-        <v>305</v>
+        <v/>
       </c>
       <c r="AC25" t="str">
-        <v>0</v>
+        <v/>
       </c>
       <c r="AD25" t="str">
-        <v>Ja</v>
+        <v/>
       </c>
       <c r="AE25" t="str">
-        <v>37367115886</v>
+        <v/>
       </c>
       <c r="AF25" t="str">
-        <v>cmkk3tb7a061qcx0137352zdc</v>
+        <v>cml0kt92t028m9e01x57iiqv1</v>
       </c>
       <c r="AG25" t="str">
         <v>Påmeldt</v>
       </c>
       <c r="AH25" t="str">
-        <v>18.01.2026</v>
+        <v/>
       </c>
       <c r="AI25" t="str">
-        <v>20:03</v>
+        <v/>
       </c>
       <c r="AJ25" t="str">
         <v>Ikke sjekket inn</v>
       </c>
       <c r="AK25" t="str">
-        <v>Betaling nr: 1 (PAID) Beløp: 305,-</v>
+        <v/>
       </c>
       <c r="AL25" t="str">
-        <v>000000000</v>
+        <v/>
       </c>
       <c r="AM25" t="str">
-        <v>9865886</v>
+        <v/>
       </c>
       <c r="AN25" t="str">
         <v/>
@@ -3675,274 +3674,12 @@
         <v>Ja</v>
       </c>
       <c r="AQ25" t="str">
-        <v>Ja</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>Aurelia</v>
-      </c>
-      <c r="B26" t="str">
-        <v>Landschulze</v>
-      </c>
-      <c r="C26" t="str">
-        <v>klandschulze@posteo.no</v>
-      </c>
-      <c r="D26" t="str">
-        <v>Tyskland</v>
-      </c>
-      <c r="E26" t="str">
-        <v>GER</v>
-      </c>
-      <c r="F26" t="str">
-        <v>10.04.2015</v>
-      </c>
-      <c r="G26" t="str">
-        <v>10 år</v>
-      </c>
-      <c r="H26" t="str">
-        <v>+4740646286</v>
-      </c>
-      <c r="I26" t="str">
-        <v>K</v>
-      </c>
-      <c r="J26" t="str">
-        <v>Fana Idrettslag</v>
-      </c>
-      <c r="K26" t="str">
-        <v>24834</v>
-      </c>
-      <c r="L26" t="str">
-        <v/>
-      </c>
-      <c r="M26" t="str">
-        <v>Hordaland Skøytekrets</v>
-      </c>
-      <c r="N26" t="str">
-        <v>878</v>
-      </c>
-      <c r="O26" t="str">
-        <v/>
-      </c>
-      <c r="P26" t="str">
-        <v/>
-      </c>
-      <c r="Q26" t="str">
-        <v xml:space="preserve">Oppvisning Reg.3 Vestlandet og Sørlandet </v>
-      </c>
-      <c r="R26" t="str">
-        <v/>
-      </c>
-      <c r="S26" t="str">
-        <v>09.02.2026</v>
-      </c>
-      <c r="T26" t="str">
-        <v>17:00</v>
-      </c>
-      <c r="U26" t="str">
-        <v>305</v>
-      </c>
-      <c r="V26" t="str">
-        <v>0</v>
-      </c>
-      <c r="W26" t="str">
-        <v>J</v>
-      </c>
-      <c r="X26" t="str">
-        <v>d1d51orf00006n01qci0</v>
-      </c>
-      <c r="Y26" t="str">
-        <v/>
-      </c>
-      <c r="Z26" t="str">
-        <v>Karin Landschulze</v>
-      </c>
-      <c r="AA26" t="str">
-        <v>klandschulze@posteo.no</v>
-      </c>
-      <c r="AB26" t="str">
-        <v>305</v>
-      </c>
-      <c r="AC26" t="str">
-        <v>0</v>
-      </c>
-      <c r="AD26" t="str">
-        <v>Ja</v>
-      </c>
-      <c r="AE26" t="str">
-        <v>37380862685</v>
-      </c>
-      <c r="AF26" t="str">
-        <v>cmklbsxxg00jycg01s2378t65</v>
-      </c>
-      <c r="AG26" t="str">
-        <v>Påmeldt</v>
-      </c>
-      <c r="AH26" t="str">
-        <v>19.01.2026</v>
-      </c>
-      <c r="AI26" t="str">
-        <v>16:34</v>
-      </c>
-      <c r="AJ26" t="str">
-        <v>Ikke sjekket inn</v>
-      </c>
-      <c r="AK26" t="str">
-        <v>Betaling nr: 1 (PAID) Beløp: 305,-</v>
-      </c>
-      <c r="AL26" t="str">
-        <v>000000000</v>
-      </c>
-      <c r="AM26" t="str">
-        <v>9583455</v>
-      </c>
-      <c r="AN26" t="str">
-        <v/>
-      </c>
-      <c r="AO26" t="str">
-        <v/>
-      </c>
-      <c r="AP26" t="str">
-        <v>Ja</v>
-      </c>
-      <c r="AQ26" t="str">
-        <v>Ja</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>Leah</v>
-      </c>
-      <c r="B27" t="str">
-        <v>Kalvik</v>
-      </c>
-      <c r="C27" t="str">
-        <v>per.asle.sandal@gmail.com</v>
-      </c>
-      <c r="D27" t="str">
-        <v>NO</v>
-      </c>
-      <c r="E27" t="str">
-        <v/>
-      </c>
-      <c r="F27" t="str">
-        <v>08.09.2014</v>
-      </c>
-      <c r="G27" t="str">
-        <v>11 år</v>
-      </c>
-      <c r="H27" t="str">
-        <v>+4741678027</v>
-      </c>
-      <c r="I27" t="str">
-        <v>K</v>
-      </c>
-      <c r="J27" t="str">
-        <v>Loddefjord IL</v>
-      </c>
-      <c r="K27" t="str">
-        <v>24878</v>
-      </c>
-      <c r="L27" t="str">
-        <v>610594</v>
-      </c>
-      <c r="M27" t="str">
-        <v>Hordaland Skøytekrets</v>
-      </c>
-      <c r="N27" t="str">
-        <v>878</v>
-      </c>
-      <c r="O27" t="str">
-        <v/>
-      </c>
-      <c r="P27" t="str">
-        <v/>
-      </c>
-      <c r="Q27" t="str">
-        <v/>
-      </c>
-      <c r="R27" t="str">
-        <v/>
-      </c>
-      <c r="S27" t="str">
-        <v>09.02.2026</v>
-      </c>
-      <c r="T27" t="str">
-        <v>17:00</v>
-      </c>
-      <c r="U27" t="str">
-        <v/>
-      </c>
-      <c r="V27" t="str">
-        <v/>
-      </c>
-      <c r="W27" t="str">
-        <v>N</v>
-      </c>
-      <c r="X27" t="str">
-        <v/>
-      </c>
-      <c r="Y27" t="str">
-        <v/>
-      </c>
-      <c r="Z27" t="str">
-        <v>Anja Papenbrock Bjarndisson</v>
-      </c>
-      <c r="AA27" t="str">
-        <v>apapenbrock@gmx.de</v>
-      </c>
-      <c r="AB27" t="str">
-        <v/>
-      </c>
-      <c r="AC27" t="str">
-        <v/>
-      </c>
-      <c r="AD27" t="str">
-        <v/>
-      </c>
-      <c r="AE27" t="str">
-        <v/>
-      </c>
-      <c r="AF27" t="str">
-        <v>cml0kt92t028m9e01x57iiqv1</v>
-      </c>
-      <c r="AG27" t="str">
-        <v>Påmeldt</v>
-      </c>
-      <c r="AH27" t="str">
-        <v/>
-      </c>
-      <c r="AI27" t="str">
-        <v/>
-      </c>
-      <c r="AJ27" t="str">
-        <v>Ikke sjekket inn</v>
-      </c>
-      <c r="AK27" t="str">
-        <v/>
-      </c>
-      <c r="AL27" t="str">
-        <v/>
-      </c>
-      <c r="AM27" t="str">
-        <v/>
-      </c>
-      <c r="AN27" t="str">
-        <v/>
-      </c>
-      <c r="AO27" t="str">
-        <v/>
-      </c>
-      <c r="AP27" t="str">
-        <v>Ja</v>
-      </c>
-      <c r="AQ27" t="str">
         <v>Nei</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AQ27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AQ25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>